<commit_message>
Updated utility classes. Factorised code.
</commit_message>
<xml_diff>
--- a/intrastat/_resources/Intrastat Data Sample.xlsx
+++ b/intrastat/_resources/Intrastat Data Sample.xlsx
@@ -40,7 +40,7 @@
     <t>Ship To</t>
   </si>
   <si>
-    <t>County of Origin</t>
+    <t>Country of Origin</t>
   </si>
   <si>
     <t>Mode of Transport</t>
@@ -578,7 +578,7 @@
     <col min="6" max="6" style="2" width="13.005" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="2" width="13.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="2" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="2" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="2" width="13.005" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="2" width="13.005" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="2" width="13.005" customWidth="1" bestFit="1"/>

</xml_diff>